<commit_message>
RMB framework with 2 curves
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/RMB_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/RMB_MainChecks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="9600" windowHeight="11955"/>
+    <workbookView xWindow="60" yWindow="15" windowWidth="19020" windowHeight="11235"/>
   </bookViews>
   <sheets>
     <sheet name="MainChecks" sheetId="2" r:id="rId1"/>
@@ -14,9 +14,9 @@
     <definedName name="FuturesTable">MainChecks!$A$10:$H$18</definedName>
     <definedName name="IMMFutures">MainChecks!#REF!</definedName>
     <definedName name="InterestRatesTrigger">MainChecks!#REF!</definedName>
-    <definedName name="OFFCurrency">MainChecks!$U$5</definedName>
+    <definedName name="OffCurrency">MainChecks!$U$5</definedName>
     <definedName name="OFFFirstIndex">MainChecks!$K$11</definedName>
-    <definedName name="ONCurrency">MainChecks!$U$4</definedName>
+    <definedName name="OnCurrency">MainChecks!$U$4</definedName>
     <definedName name="ONFirstIndex">MainChecks!$K$10</definedName>
     <definedName name="TenYearsBondFutures">MainChecks!$C$10:$C$12</definedName>
     <definedName name="Trigger">MainChecks!$U$2</definedName>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
   <si>
     <t>ObjectID</t>
   </si>
@@ -749,34 +749,34 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 11:41:46</v>
+        <v>Paused at 16:40:09</v>
         <stp/>
-        <stp>{85BC0E35-D8F8-42CA-A9EF-C6699D75719B}</stp>
+        <stp>{78BA36F5-D401-4859-95E4-B9AAADB77244}</stp>
+        <tr r="P6" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Paused at 16:40:09</v>
+        <stp/>
+        <stp>{05C746D1-1489-437C-89DF-BBE3F2779878}</stp>
         <tr r="Q6" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 11:41:46</v>
+        <v>Paused at 16:40:09</v>
         <stp/>
-        <stp>{99129A87-6CB9-4509-A1D9-6ABBEACBFCAC}</stp>
-        <tr r="P6" s="2"/>
+        <stp>{2B3462EC-92A6-4AC5-9CCA-85FF4950E140}</stp>
+        <tr r="Q5" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 15:42:26</v>
+        <v>Paused at 16:40:09</v>
         <stp/>
-        <stp>{93051578-7274-44A7-B12C-699F864637A6}</stp>
+        <stp>{C3AABF72-2308-40BF-9990-87053CC4E3F3}</stp>
         <tr r="Q7" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 15:42:26</v>
+        <v>Paused at 16:40:09</v>
         <stp/>
-        <stp>{6BECB31D-E40F-41A3-81AF-2CF609EB15E3}</stp>
+        <stp>{7EE1FAD1-3D6C-457C-85FF-1580EEB8847E}</stp>
         <tr r="P7" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 16:01:01</v>
-        <stp/>
-        <stp>{C8AB787B-3944-4E0E-8765-3F7B9169217A}</stp>
-        <tr r="Q5" s="2"/>
       </tp>
     </main>
   </volType>
@@ -1390,14 +1390,14 @@
         <v>41981</v>
       </c>
       <c r="M5" s="27">
-        <v>149.31</v>
+        <v>147.84</v>
       </c>
       <c r="N5" s="27"/>
       <c r="O5" s="27"/>
       <c r="P5" s="27"/>
       <c r="Q5" s="28" t="str">
         <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>Updated at 16:01:01</v>
+        <v>Paused at 16:40:09</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>12</v>
@@ -1437,29 +1437,29 @@
       <c r="I6" s="3"/>
       <c r="J6" s="21"/>
       <c r="K6" s="22" t="str">
-        <f>ONCurrency&amp;VLOOKUP(ONCurrency,FuturesTable,5,0)&amp;VLOOKUP(ONCurrency,FuturesTable,6,0)&amp;"10Y"</f>
+        <f>OnCurrency&amp;VLOOKUP(OnCurrency,FuturesTable,5,0)&amp;VLOOKUP(OnCurrency,FuturesTable,6,0)&amp;"10Y"</f>
         <v>CNYQM3S10Y</v>
       </c>
       <c r="L6" s="23">
-        <v>41880</v>
+        <v>41900</v>
       </c>
       <c r="M6" s="31" t="str">
         <f>N6&amp;"/"&amp;O6</f>
-        <v>4.36/4.56</v>
+        <v>4.13/4.33</v>
       </c>
       <c r="N6" s="29">
-        <v>4.3600000000000003</v>
+        <v>4.13</v>
       </c>
       <c r="O6" s="29">
-        <v>4.5599999999999996</v>
+        <v>4.33</v>
       </c>
       <c r="P6" s="29" t="str">
-        <f>_xll.RData(K6&amp;"="&amp;VLOOKUP(ONCurrency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N6)</f>
-        <v>Updated at 11:41:46</v>
+        <f>_xll.RData(K6&amp;"="&amp;VLOOKUP(OnCurrency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N6)</f>
+        <v>Paused at 16:40:09</v>
       </c>
       <c r="Q6" s="30" t="str">
-        <f>_xll.RData(K6&amp;"="&amp;VLOOKUP(ONCurrency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L6)</f>
-        <v>Updated at 11:41:46</v>
+        <f>_xll.RData(K6&amp;"="&amp;VLOOKUP(OnCurrency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L6)</f>
+        <v>Paused at 16:40:09</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>12</v>
@@ -1500,7 +1500,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="21"/>
       <c r="K7" s="22" t="str">
-        <f>OFFCurrency&amp;VLOOKUP(OFFCurrency,FuturesTable,5,0)&amp;VLOOKUP(OFFCurrency,FuturesTable,6,0)&amp;"10Y"</f>
+        <f>OffCurrency&amp;VLOOKUP(OffCurrency,FuturesTable,5,0)&amp;VLOOKUP(OffCurrency,FuturesTable,6,0)&amp;"10Y"</f>
         <v>CNHQM3H10Y</v>
       </c>
       <c r="L7" s="23">
@@ -1517,12 +1517,12 @@
         <v>0</v>
       </c>
       <c r="P7" s="29" t="str">
-        <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(ONCurrency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N7)</f>
-        <v>Updated at 15:42:26</v>
+        <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(OnCurrency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N7)</f>
+        <v>Paused at 16:40:09</v>
       </c>
       <c r="Q7" s="30" t="str">
-        <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(ONCurrency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L7)</f>
-        <v>Updated at 15:42:26</v>
+        <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(OnCurrency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L7)</f>
+        <v>Paused at 16:40:09</v>
       </c>
       <c r="R7" s="8"/>
       <c r="S7" s="1"/>
@@ -1531,7 +1531,7 @@
       </c>
       <c r="U7" s="12">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>500</v>
+        <v>281</v>
       </c>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
@@ -1667,16 +1667,16 @@
       <c r="I10" s="3"/>
       <c r="J10" s="7"/>
       <c r="K10" s="25" t="str">
-        <f>PROPER(ONCurrency)&amp;VLOOKUP(ONCurrency,FuturesTable,8,0)&amp;VLOOKUP(ONCurrency,FuturesTable,2,0)</f>
+        <f>PROPER(OnCurrency)&amp;VLOOKUP(OnCurrency,FuturesTable,8,0)&amp;VLOOKUP(OnCurrency,FuturesTable,2,0)</f>
         <v>CnyShibor3M</v>
       </c>
       <c r="L10" s="26">
         <f>_xll.qlLastFixingQuoteReferenceDate(ONFirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>41887</v>
+        <v>41900</v>
       </c>
       <c r="M10" s="38">
         <f>_xll.qlQuoteValue(ONFirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>4.6539000000000004E-2</v>
+        <v>4.6205999999999997E-2</v>
       </c>
       <c r="N10" s="38"/>
       <c r="O10" s="38"/>
@@ -1735,16 +1735,16 @@
       <c r="I11" s="3"/>
       <c r="J11" s="7"/>
       <c r="K11" s="40" t="str">
-        <f>PROPER(OFFCurrency)&amp;VLOOKUP(OFFCurrency,FuturesTable,8,0)&amp;VLOOKUP(OFFCurrency,FuturesTable,2,0)</f>
+        <f>PROPER(OffCurrency)&amp;VLOOKUP(OffCurrency,FuturesTable,8,0)&amp;VLOOKUP(OffCurrency,FuturesTable,2,0)</f>
         <v>CnhHibor3M</v>
       </c>
       <c r="L11" s="41">
         <f>_xll.qlLastFixingQuoteReferenceDate(OFFFirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>41890</v>
+        <v>41900</v>
       </c>
       <c r="M11" s="42">
         <f>_xll.qlQuoteValue(OFFFirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>3.1244399999999999E-2</v>
+        <v>3.3594400000000003E-2</v>
       </c>
       <c r="N11" s="42"/>
       <c r="O11" s="42"/>
@@ -1753,7 +1753,9 @@
         <f>IF(AND(ISERROR(L11),ISERROR(M11)),_xll.ohRangeRetrieveError(L11)&amp;" "&amp;_xll.ohRangeRetrieveError(M11),IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11)))</f>
         <v/>
       </c>
-      <c r="R11" s="8"/>
+      <c r="R11" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
@@ -1801,7 +1803,7 @@
       <c r="I12" s="3"/>
       <c r="J12" s="7"/>
       <c r="K12" s="25" t="str">
-        <f>UPPER(ONCurrency)&amp;"7DREPO"</f>
+        <f>UPPER(OnCurrency)&amp;"7DREPO"</f>
         <v>CNY7DREPO</v>
       </c>
       <c r="L12" s="26" t="e">
@@ -1867,7 +1869,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="7"/>
       <c r="K13" s="22" t="str">
-        <f>UPPER(ONCurrency)&amp;"7DREPOND"</f>
+        <f>UPPER(OnCurrency)&amp;"7DREPOND"</f>
         <v>CNY7DREPOND</v>
       </c>
       <c r="L13" s="23" t="e">
@@ -1933,23 +1935,23 @@
       <c r="I14" s="3"/>
       <c r="J14" s="7"/>
       <c r="K14" s="22" t="str">
-        <f>UPPER(ONCurrency)&amp;"3M"</f>
+        <f>UPPER(OnCurrency)&amp;"3M"</f>
         <v>CNY3M</v>
       </c>
-      <c r="L14" s="23">
+      <c r="L14" s="23" t="e">
         <f>_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
-        <v>41891</v>
-      </c>
-      <c r="M14" s="24">
+        <v>#NUM!</v>
+      </c>
+      <c r="M14" s="24" t="e">
         <f>_xll.qlYieldTSDiscount(K14,L14)</f>
-        <v>1</v>
+        <v>#NUM!</v>
       </c>
       <c r="N14" s="24"/>
       <c r="O14" s="24"/>
       <c r="P14" s="24"/>
       <c r="Q14" s="32" t="str">
-        <f>IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
-        <v/>
+        <f ca="1">IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
+        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
       </c>
       <c r="R14" s="8" t="s">
         <v>12</v>
@@ -1999,7 +2001,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="7"/>
       <c r="K15" s="22" t="str">
-        <f>UPPER(ONCurrency)&amp;"ON"</f>
+        <f>UPPER(OnCurrency)&amp;"ON"</f>
         <v>CNYON</v>
       </c>
       <c r="L15" s="23" t="e">
@@ -2065,7 +2067,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="7"/>
       <c r="K16" s="22" t="str">
-        <f>UPPER(ONCurrency)&amp;"1Y"</f>
+        <f>UPPER(OnCurrency)&amp;"1Y"</f>
         <v>CNY1Y</v>
       </c>
       <c r="L16" s="23" t="e">
@@ -2131,23 +2133,23 @@
       <c r="I17" s="3"/>
       <c r="J17" s="7"/>
       <c r="K17" s="40" t="str">
-        <f>UPPER(OFFCurrency)&amp;"3M"</f>
+        <f>UPPER(OffCurrency)&amp;"3M"</f>
         <v>CNH3M</v>
       </c>
-      <c r="L17" s="41">
+      <c r="L17" s="41" t="e">
         <f>_xll.qlTermStructureReferenceDate(K17,Trigger)</f>
-        <v>41893</v>
-      </c>
-      <c r="M17" s="46">
+        <v>#NUM!</v>
+      </c>
+      <c r="M17" s="46" t="e">
         <f>_xll.qlYieldTSDiscount(K17,L17)</f>
-        <v>1</v>
+        <v>#NUM!</v>
       </c>
       <c r="N17" s="46"/>
       <c r="O17" s="46"/>
       <c r="P17" s="46"/>
       <c r="Q17" s="47" t="str">
-        <f>IF(ISERROR(L17),_xll.ohRangeRetrieveError(L17),_xll.ohRangeRetrieveError(M17))</f>
-        <v/>
+        <f ca="1">IF(ISERROR(L17),_xll.ohRangeRetrieveError(L17),_xll.ohRangeRetrieveError(M17))</f>
+        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
       </c>
       <c r="R17" s="8" t="s">
         <v>12</v>
@@ -5390,7 +5392,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="CommandButton2">
+        <control shapeId="1025" r:id="rId4" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5410,12 +5412,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="CommandButton2"/>
+        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId6" name="CommandButton1">
+        <control shapeId="1026" r:id="rId6" name="CommandButton2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5435,7 +5437,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId6" name="CommandButton1"/>
+        <control shapeId="1026" r:id="rId6" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
RMB framework with 7D Curves
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/RMB_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/RMB_MainChecks.xlsx
@@ -749,34 +749,34 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Paused at 16:40:09</v>
+        <v>Updated at 16:36:49</v>
         <stp/>
-        <stp>{78BA36F5-D401-4859-95E4-B9AAADB77244}</stp>
-        <tr r="P6" s="2"/>
+        <stp>{9264430A-1137-4C6F-9305-AFA4CCCB0162}</stp>
+        <tr r="P7" s="2"/>
       </tp>
       <tp t="s">
-        <v>Paused at 16:40:09</v>
+        <v>Updated at 16:36:49</v>
         <stp/>
-        <stp>{05C746D1-1489-437C-89DF-BBE3F2779878}</stp>
+        <stp>{63201497-0305-47F5-9DCE-E7C1859F7586}</stp>
+        <tr r="Q7" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 16:37:23</v>
+        <stp/>
+        <stp>{C5EF1BC9-466C-4A64-9D85-DD410C240FEF}</stp>
+        <tr r="Q5" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 16:36:46</v>
+        <stp/>
+        <stp>{7AA5AF5E-9BC9-43D9-AB68-87EE2809B077}</stp>
         <tr r="Q6" s="2"/>
       </tp>
       <tp t="s">
-        <v>Paused at 16:40:09</v>
+        <v>Updated at 16:36:46</v>
         <stp/>
-        <stp>{2B3462EC-92A6-4AC5-9CCA-85FF4950E140}</stp>
-        <tr r="Q5" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Paused at 16:40:09</v>
-        <stp/>
-        <stp>{C3AABF72-2308-40BF-9990-87053CC4E3F3}</stp>
-        <tr r="Q7" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Paused at 16:40:09</v>
-        <stp/>
-        <stp>{7EE1FAD1-3D6C-457C-85FF-1580EEB8847E}</stp>
-        <tr r="P7" s="2"/>
+        <stp>{3E9CB8BB-9B1C-41D9-B705-31DF53A6BCCD}</stp>
+        <tr r="P6" s="2"/>
       </tp>
     </main>
   </volType>
@@ -1384,20 +1384,20 @@
       <c r="I5" s="3"/>
       <c r="J5" s="7"/>
       <c r="K5" s="25" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="L5" s="26">
-        <v>41981</v>
+        <v>41992</v>
       </c>
       <c r="M5" s="27">
-        <v>147.84</v>
+        <v>125.25</v>
       </c>
       <c r="N5" s="27"/>
       <c r="O5" s="27"/>
       <c r="P5" s="27"/>
       <c r="Q5" s="28" t="str">
         <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>Paused at 16:40:09</v>
+        <v>Updated at 16:37:23</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>12</v>
@@ -1437,29 +1437,29 @@
       <c r="I6" s="3"/>
       <c r="J6" s="21"/>
       <c r="K6" s="22" t="str">
-        <f>OnCurrency&amp;VLOOKUP(OnCurrency,FuturesTable,5,0)&amp;VLOOKUP(OnCurrency,FuturesTable,6,0)&amp;"10Y"</f>
-        <v>CNYQM3S10Y</v>
+        <f>OnCurrency&amp;VLOOKUP(OnCurrency,FuturesTable,5,0)&amp;VLOOKUP(OnCurrency,FuturesTable,6,0)&amp;"1Y"</f>
+        <v>CNYQM3S1Y</v>
       </c>
       <c r="L6" s="23">
-        <v>41900</v>
+        <v>41912</v>
       </c>
       <c r="M6" s="31" t="str">
         <f>N6&amp;"/"&amp;O6</f>
-        <v>4.13/4.33</v>
+        <v>4/4.2</v>
       </c>
       <c r="N6" s="29">
-        <v>4.13</v>
+        <v>4</v>
       </c>
       <c r="O6" s="29">
-        <v>4.33</v>
+        <v>4.2</v>
       </c>
       <c r="P6" s="29" t="str">
         <f>_xll.RData(K6&amp;"="&amp;VLOOKUP(OnCurrency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N6)</f>
-        <v>Paused at 16:40:09</v>
+        <v>Updated at 16:36:46</v>
       </c>
       <c r="Q6" s="30" t="str">
         <f>_xll.RData(K6&amp;"="&amp;VLOOKUP(OnCurrency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L6)</f>
-        <v>Paused at 16:40:09</v>
+        <v>Updated at 16:36:46</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>12</v>
@@ -1500,29 +1500,29 @@
       <c r="I7" s="3"/>
       <c r="J7" s="21"/>
       <c r="K7" s="22" t="str">
-        <f>OffCurrency&amp;VLOOKUP(OffCurrency,FuturesTable,5,0)&amp;VLOOKUP(OffCurrency,FuturesTable,6,0)&amp;"10Y"</f>
-        <v>CNHQM3H10Y</v>
+        <f>OffCurrency&amp;VLOOKUP(OffCurrency,FuturesTable,5,0)&amp;VLOOKUP(OffCurrency,FuturesTable,6,0)&amp;"1Y"</f>
+        <v>CNHQM3H1Y</v>
       </c>
       <c r="L7" s="23">
-        <v>41474</v>
+        <v>41918</v>
       </c>
       <c r="M7" s="31" t="str">
         <f>N7&amp;"/"&amp;O7</f>
-        <v>2.9/0</v>
+        <v>3.2/3.3</v>
       </c>
       <c r="N7" s="29">
-        <v>2.9</v>
+        <v>3.2</v>
       </c>
       <c r="O7" s="29">
-        <v>0</v>
+        <v>3.3000000000000003</v>
       </c>
       <c r="P7" s="29" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(OnCurrency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N7)</f>
-        <v>Paused at 16:40:09</v>
+        <v>Updated at 16:36:49</v>
       </c>
       <c r="Q7" s="30" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(OnCurrency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L7)</f>
-        <v>Paused at 16:40:09</v>
+        <v>Updated at 16:36:49</v>
       </c>
       <c r="R7" s="8"/>
       <c r="S7" s="1"/>
@@ -1531,7 +1531,7 @@
       </c>
       <c r="U7" s="12">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>281</v>
+        <v>637</v>
       </c>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
@@ -1672,11 +1672,11 @@
       </c>
       <c r="L10" s="26">
         <f>_xll.qlLastFixingQuoteReferenceDate(ONFirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>41900</v>
+        <v>41912</v>
       </c>
       <c r="M10" s="38">
         <f>_xll.qlQuoteValue(ONFirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>4.6205999999999997E-2</v>
+        <v>4.5444999999999999E-2</v>
       </c>
       <c r="N10" s="38"/>
       <c r="O10" s="38"/>
@@ -1740,18 +1740,18 @@
       </c>
       <c r="L11" s="41">
         <f>_xll.qlLastFixingQuoteReferenceDate(OFFFirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>41900</v>
-      </c>
-      <c r="M11" s="42">
+        <v>41918</v>
+      </c>
+      <c r="M11" s="42" t="e">
         <f>_xll.qlQuoteValue(OFFFirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>3.3594400000000003E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="N11" s="42"/>
       <c r="O11" s="42"/>
       <c r="P11" s="42"/>
       <c r="Q11" s="43" t="str">
-        <f>IF(AND(ISERROR(L11),ISERROR(M11)),_xll.ohRangeRetrieveError(L11)&amp;" "&amp;_xll.ohRangeRetrieveError(M11),IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11)))</f>
-        <v/>
+        <f ca="1">IF(AND(ISERROR(L11),ISERROR(M11)),_xll.ohRangeRetrieveError(L11)&amp;" "&amp;_xll.ohRangeRetrieveError(M11),IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11)))</f>
+        <v>qlQuoteValue - null term structure set to this instance of HiborSN Actual/365 (Fixed)</v>
       </c>
       <c r="R11" s="8" t="s">
         <v>12</v>
@@ -1803,23 +1803,23 @@
       <c r="I12" s="3"/>
       <c r="J12" s="7"/>
       <c r="K12" s="25" t="str">
-        <f>UPPER(OnCurrency)&amp;"7DREPO"</f>
-        <v>CNY7DREPO</v>
-      </c>
-      <c r="L12" s="26" t="e">
+        <f>UPPER(OnCurrency)&amp;"7D"</f>
+        <v>CNY7D</v>
+      </c>
+      <c r="L12" s="26">
         <f>_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M12" s="44" t="e">
+        <v>41920</v>
+      </c>
+      <c r="M12" s="44">
         <f>_xll.qlYieldTSDiscount(K12,L12)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="N12" s="44"/>
       <c r="O12" s="44"/>
       <c r="P12" s="44"/>
       <c r="Q12" s="45" t="str">
-        <f ca="1">IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
-        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
+        <f>IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
+        <v/>
       </c>
       <c r="R12" s="8" t="s">
         <v>12</v>
@@ -1869,23 +1869,23 @@
       <c r="I13" s="3"/>
       <c r="J13" s="7"/>
       <c r="K13" s="22" t="str">
-        <f>UPPER(OnCurrency)&amp;"7DREPOND"</f>
-        <v>CNY7DREPOND</v>
-      </c>
-      <c r="L13" s="23" t="e">
+        <f>UPPER(OnCurrency)&amp;"7DND"</f>
+        <v>CNY7DND</v>
+      </c>
+      <c r="L13" s="23">
         <f>_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M13" s="24" t="e">
+        <v>41920</v>
+      </c>
+      <c r="M13" s="24">
         <f>_xll.qlYieldTSDiscount(K13,L13)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="N13" s="24"/>
       <c r="O13" s="24"/>
       <c r="P13" s="24"/>
       <c r="Q13" s="32" t="str">
-        <f ca="1">IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
-        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID 'CNY7DREPOND'</v>
+        <f>IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
+        <v/>
       </c>
       <c r="R13" s="8" t="s">
         <v>12</v>
@@ -1938,20 +1938,20 @@
         <f>UPPER(OnCurrency)&amp;"3M"</f>
         <v>CNY3M</v>
       </c>
-      <c r="L14" s="23" t="e">
+      <c r="L14" s="23">
         <f>_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M14" s="24" t="e">
+        <v>41912</v>
+      </c>
+      <c r="M14" s="24">
         <f>_xll.qlYieldTSDiscount(K14,L14)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="N14" s="24"/>
       <c r="O14" s="24"/>
       <c r="P14" s="24"/>
       <c r="Q14" s="32" t="str">
-        <f ca="1">IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
-        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
+        <f>IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
+        <v/>
       </c>
       <c r="R14" s="8" t="s">
         <v>12</v>
@@ -2017,7 +2017,7 @@
       <c r="P15" s="24"/>
       <c r="Q15" s="32" t="str">
         <f ca="1">IF(ISERROR(L15),_xll.ohRangeRetrieveError(L15),_xll.ohRangeRetrieveError(M15))</f>
-        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID 'CNYON'</v>
+        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
       </c>
       <c r="R15" s="8" t="s">
         <v>12</v>
@@ -2083,7 +2083,7 @@
       <c r="P16" s="24"/>
       <c r="Q16" s="32" t="str">
         <f ca="1">IF(ISERROR(L16),_xll.ohRangeRetrieveError(L16),_xll.ohRangeRetrieveError(M16))</f>
-        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID 'CNY1Y'</v>
+        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
       </c>
       <c r="R16" s="8" t="s">
         <v>12</v>
@@ -2136,20 +2136,20 @@
         <f>UPPER(OffCurrency)&amp;"3M"</f>
         <v>CNH3M</v>
       </c>
-      <c r="L17" s="41" t="e">
+      <c r="L17" s="41">
         <f>_xll.qlTermStructureReferenceDate(K17,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M17" s="46" t="e">
+        <v>41918</v>
+      </c>
+      <c r="M17" s="46">
         <f>_xll.qlYieldTSDiscount(K17,L17)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="N17" s="46"/>
       <c r="O17" s="46"/>
       <c r="P17" s="46"/>
       <c r="Q17" s="47" t="str">
-        <f ca="1">IF(ISERROR(L17),_xll.ohRangeRetrieveError(L17),_xll.ohRangeRetrieveError(M17))</f>
-        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
+        <f>IF(ISERROR(L17),_xll.ohRangeRetrieveError(L17),_xll.ohRangeRetrieveError(M17))</f>
+        <v/>
       </c>
       <c r="R17" s="8" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
RMB Framework with HK suggestions
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/RMB_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/RMB_MainChecks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="15" windowWidth="19020" windowHeight="11235"/>
+    <workbookView minimized="1" xWindow="28605" yWindow="-15" windowWidth="9615" windowHeight="9810"/>
   </bookViews>
   <sheets>
     <sheet name="MainChecks" sheetId="2" r:id="rId1"/>
@@ -15,9 +15,10 @@
     <definedName name="IMMFutures">MainChecks!#REF!</definedName>
     <definedName name="InterestRatesTrigger">MainChecks!#REF!</definedName>
     <definedName name="OffCurrency">MainChecks!$U$5</definedName>
-    <definedName name="OFFFirstIndex">MainChecks!$K$11</definedName>
+    <definedName name="OFFFirstIndex">MainChecks!$K$12</definedName>
     <definedName name="OnCurrency">MainChecks!$U$4</definedName>
-    <definedName name="ONFirstIndex">MainChecks!$K$10</definedName>
+    <definedName name="ONFirstIndex">MainChecks!$K$11</definedName>
+    <definedName name="ONIndex">MainChecks!$K$10</definedName>
     <definedName name="TenYearsBondFutures">MainChecks!$C$4:$C$12</definedName>
     <definedName name="Trigger">MainChecks!$U$2</definedName>
   </definedNames>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="58">
   <si>
     <t>ObjectID</t>
   </si>
@@ -545,7 +546,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -666,6 +667,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="1"/>
@@ -764,34 +771,36 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Paused at 17:16:50</v>
+        <v>Updated at 12:46:28</v>
         <stp/>
-        <stp>{11FE63BE-DA9B-4087-B220-0A58D5BCB057}</stp>
+        <stp>{366730A4-B07F-43D6-A64A-4A85339EAD13}</stp>
+        <tr r="Q5" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 12:41:08</v>
+        <stp/>
+        <stp>{AD13145B-9768-4F71-B411-AEDA3393E5ED}</stp>
+        <tr r="Q7" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 12:41:08</v>
+        <stp/>
+        <stp>{1244A927-E79D-4CA5-8CC0-A8D987EFFF9F}</stp>
         <tr r="P6" s="2"/>
       </tp>
       <tp t="s">
-        <v>Paused at 17:16:50</v>
+        <v>Updated at 12:41:08</v>
         <stp/>
-        <stp>{D5E9C787-754A-4602-9EEB-D5EC104E7BD0}</stp>
-        <tr r="P7" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Paused at 17:16:50</v>
-        <stp/>
-        <stp>{D9FE9393-CE5F-4C34-A0C4-5966D49020E5}</stp>
+        <stp>{BC0E8360-EE5B-41D0-8DDA-5F51DAF2E15E}</stp>
         <tr r="Q6" s="2"/>
       </tp>
+    </main>
+    <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Paused at 17:16:50</v>
+        <v>Updated at 12:41:08</v>
         <stp/>
-        <stp>{9C359F13-8CA4-49D9-8AEF-98229A3332C6}</stp>
-        <tr r="Q7" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Paused at 17:16:50</v>
-        <stp/>
-        <stp>{158CE45F-3CDF-4E88-B4E2-192C2DF10DFD}</stp>
-        <tr r="Q5" s="2"/>
+        <stp>{695A927E-CF5C-4A5C-B19E-2EACA98AFF14}</stp>
+        <tr r="P7" s="2"/>
       </tp>
     </main>
   </volType>
@@ -1276,9 +1285,7 @@
       <c r="T2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="18">
-        <v>41919.7190162037</v>
-      </c>
+      <c r="U2" s="18"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
@@ -1440,14 +1447,14 @@
         <v>41992</v>
       </c>
       <c r="M5" s="26">
-        <v>125.78125</v>
+        <v>126.078125</v>
       </c>
       <c r="N5" s="26"/>
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
       <c r="Q5" s="27" t="str">
         <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>Paused at 17:16:50</v>
+        <v>Updated at 12:46:28</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>12</v>
@@ -1521,11 +1528,11 @@
       </c>
       <c r="P6" s="28" t="str">
         <f>_xll.RData(K6&amp;"="&amp;VLOOKUP(OnCurrency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N6)</f>
-        <v>Paused at 17:16:50</v>
+        <v>Updated at 12:41:08</v>
       </c>
       <c r="Q6" s="29" t="str">
         <f>_xll.RData(K6&amp;"="&amp;VLOOKUP(OnCurrency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L6)</f>
-        <v>Paused at 17:16:50</v>
+        <v>Updated at 12:41:08</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>12</v>
@@ -1600,11 +1607,11 @@
       </c>
       <c r="P7" s="28" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(OnCurrency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N7)</f>
-        <v>Paused at 17:16:50</v>
+        <v>Updated at 12:41:08</v>
       </c>
       <c r="Q7" s="29" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(OnCurrency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L7)</f>
-        <v>Paused at 17:16:50</v>
+        <v>Updated at 12:41:08</v>
       </c>
       <c r="R7" s="8"/>
       <c r="S7" s="1"/>
@@ -1613,7 +1620,7 @@
       </c>
       <c r="U7" s="11">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>651</v>
+        <v>582</v>
       </c>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
@@ -1781,16 +1788,16 @@
       <c r="I10" s="3"/>
       <c r="J10" s="7"/>
       <c r="K10" s="24" t="str">
-        <f>PROPER(OnCurrency)&amp;VLOOKUP(OnCurrency,FuturesTable,8,0)&amp;VLOOKUP(OnCurrency,FuturesTable,2,0)</f>
-        <v>CnyShibor3M</v>
+        <f>PROPER(OnCurrency)&amp;"Repo7D"</f>
+        <v>CnyRepo7D</v>
       </c>
       <c r="L10" s="25">
-        <f>_xll.qlLastFixingQuoteReferenceDate(ONFirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>41912</v>
+        <f>_xll.qlLastFixingQuoteReferenceDate(ONIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>41920</v>
       </c>
       <c r="M10" s="33">
-        <f>_xll.qlQuoteValue(ONFirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>4.5444999999999999E-2</v>
+        <f>_xll.qlQuoteValue(ONIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>3.0900000000000004E-2</v>
       </c>
       <c r="N10" s="33"/>
       <c r="O10" s="33"/>
@@ -1848,28 +1855,26 @@
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="7"/>
-      <c r="K11" s="35" t="str">
-        <f>PROPER(OffCurrency)&amp;VLOOKUP(OffCurrency,FuturesTable,8,0)&amp;VLOOKUP(OffCurrency,FuturesTable,2,0)</f>
-        <v>CnhHibor3M</v>
-      </c>
-      <c r="L11" s="36">
-        <f>_xll.qlLastFixingQuoteReferenceDate(OFFFirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>41919</v>
-      </c>
-      <c r="M11" s="37">
-        <f>_xll.qlQuoteValue(OFFFirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>2.7950000000000003E-2</v>
-      </c>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
-      <c r="P11" s="37"/>
-      <c r="Q11" s="38" t="str">
+      <c r="K11" s="21" t="str">
+        <f>PROPER(OnCurrency)&amp;VLOOKUP(OnCurrency,FuturesTable,8,0)&amp;VLOOKUP(OnCurrency,FuturesTable,2,0)</f>
+        <v>CnyShibor3M</v>
+      </c>
+      <c r="L11" s="22">
+        <f>_xll.qlLastFixingQuoteReferenceDate(ONFirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>41920</v>
+      </c>
+      <c r="M11" s="54">
+        <f>_xll.qlQuoteValue(ONFirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>4.5440000000000008E-2</v>
+      </c>
+      <c r="N11" s="54"/>
+      <c r="O11" s="54"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="55" t="str">
         <f>IF(AND(ISERROR(L11),ISERROR(M11)),_xll.ohRangeRetrieveError(L11)&amp;" "&amp;_xll.ohRangeRetrieveError(M11),IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11)))</f>
         <v/>
       </c>
-      <c r="R11" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="R11" s="8"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
@@ -1910,23 +1915,23 @@
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="24" t="str">
-        <f>UPPER(OnCurrency)&amp;"7D"</f>
-        <v>CNY7D</v>
-      </c>
-      <c r="L12" s="25">
-        <f>_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
+      <c r="K12" s="35" t="str">
+        <f>PROPER(OffCurrency)&amp;VLOOKUP(OffCurrency,FuturesTable,8,0)&amp;VLOOKUP(OffCurrency,FuturesTable,2,0)</f>
+        <v>CnhHibor3M</v>
+      </c>
+      <c r="L12" s="36">
+        <f>_xll.qlLastFixingQuoteReferenceDate(OFFFirstIndex&amp;"LastFixing_Quote",Trigger)</f>
         <v>41920</v>
       </c>
-      <c r="M12" s="39">
-        <f>_xll.qlYieldTSDiscount(K12,L12)</f>
-        <v>1</v>
-      </c>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="40" t="str">
-        <f>IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
+      <c r="M12" s="37">
+        <f>_xll.qlQuoteValue(OFFFirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>3.2900000000000006E-2</v>
+      </c>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="38" t="str">
+        <f>IF(AND(ISERROR(L12),ISERROR(M12)),_xll.ohRangeRetrieveError(L12)&amp;" "&amp;_xll.ohRangeRetrieveError(M12),IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12)))</f>
         <v/>
       </c>
       <c r="R12" s="8" t="s">
@@ -1962,22 +1967,22 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="21" t="str">
-        <f>UPPER(OnCurrency)&amp;"7DND"</f>
-        <v>CNY7DND</v>
-      </c>
-      <c r="L13" s="22">
+      <c r="K13" s="24" t="str">
+        <f>UPPER(OnCurrency)&amp;"7D"</f>
+        <v>CNY7D</v>
+      </c>
+      <c r="L13" s="25">
         <f>_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
-        <v>41920</v>
-      </c>
-      <c r="M13" s="23">
+        <v>41921</v>
+      </c>
+      <c r="M13" s="39">
         <f>_xll.qlYieldTSDiscount(K13,L13)</f>
         <v>1</v>
       </c>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="31" t="str">
+      <c r="N13" s="39"/>
+      <c r="O13" s="39"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="40" t="str">
         <f>IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
         <v/>
       </c>
@@ -2176,7 +2181,7 @@
       </c>
       <c r="L17" s="36">
         <f>_xll.qlTermStructureReferenceDate(K17,Trigger)</f>
-        <v>41921</v>
+        <v>41922</v>
       </c>
       <c r="M17" s="41">
         <f>_xll.qlYieldTSDiscount(K17,L17)</f>
@@ -5404,7 +5409,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U4:U5">
       <formula1>"EUR,USD,GBP,JPY,CHF,AUD,CNY,CNH,HKD"</formula1>
     </dataValidation>
@@ -5417,7 +5422,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="CommandButton2">
+        <control shapeId="1025" r:id="rId4" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5437,12 +5442,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="CommandButton2"/>
+        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId6" name="CommandButton1">
+        <control shapeId="1026" r:id="rId6" name="CommandButton2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5462,7 +5467,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId6" name="CommandButton1"/>
+        <control shapeId="1026" r:id="rId6" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>